<commit_message>
cambios a la estructura de las tablas
</commit_message>
<xml_diff>
--- a/Documentación/Casos de Prueba.xlsx
+++ b/Documentación/Casos de Prueba.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Casos ID</t>
   </si>
@@ -259,11 +259,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -591,20 +596,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="61.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="61.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="77" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="31.375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -618,13 +623,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18">
+    <row r="2" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" ht="18">
+    <row r="3" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -638,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18">
+    <row r="4" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -652,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18">
+    <row r="5" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -666,7 +671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="36">
+    <row r="6" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -680,7 +685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="36">
+    <row r="7" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -694,7 +699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="36">
+    <row r="8" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -708,7 +713,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="36">
+    <row r="9" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -722,7 +727,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="54">
+    <row r="10" spans="1:4" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -732,9 +737,11 @@
       <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" ht="36">
+      <c r="D10" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -748,7 +755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="36">
+    <row r="12" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -762,7 +769,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="54">
+    <row r="13" spans="1:4" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -776,7 +783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="36">
+    <row r="14" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -790,7 +797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="36">
+    <row r="15" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -804,7 +811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="54">
+    <row r="16" spans="1:4" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -818,7 +825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="36">
+    <row r="17" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -832,7 +839,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="72">
+    <row r="18" spans="1:4" ht="81" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -846,7 +853,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="54">
+    <row r="19" spans="1:4" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -860,7 +867,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="72">
+    <row r="20" spans="1:4" ht="81" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -874,7 +881,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="54">
+    <row r="21" spans="1:4" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -888,7 +895,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="36">
+    <row r="22" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -902,7 +909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18">
+    <row r="23" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -910,7 +917,7 @@
       <c r="C23" s="4"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" ht="18">
+    <row r="24" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -918,7 +925,7 @@
       <c r="C24" s="4"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="18">
+    <row r="25" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -926,7 +933,7 @@
       <c r="C25" s="4"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" ht="18">
+    <row r="26" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -934,7 +941,7 @@
       <c r="C26" s="4"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" ht="18">
+    <row r="27" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -942,7 +949,7 @@
       <c r="C27" s="4"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="18">
+    <row r="28" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -950,7 +957,7 @@
       <c r="C28" s="4"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="18">
+    <row r="29" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -958,7 +965,7 @@
       <c r="C29" s="4"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="18">
+    <row r="30" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -966,7 +973,7 @@
       <c r="C30" s="4"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" ht="18">
+    <row r="31" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -974,7 +981,7 @@
       <c r="C31" s="4"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="18">
+    <row r="32" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -982,7 +989,7 @@
       <c r="C32" s="4"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="18">
+    <row r="33" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -990,7 +997,7 @@
       <c r="C33" s="4"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" ht="18">
+    <row r="34" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -998,7 +1005,7 @@
       <c r="C34" s="4"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="18">
+    <row r="35" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -1006,7 +1013,7 @@
       <c r="C35" s="4"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="18">
+    <row r="36" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -1014,7 +1021,7 @@
       <c r="C36" s="4"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" ht="18">
+    <row r="37" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -1022,7 +1029,7 @@
       <c r="C37" s="4"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" ht="18">
+    <row r="38" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -1030,7 +1037,7 @@
       <c r="C38" s="4"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" ht="18">
+    <row r="39" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -1038,7 +1045,7 @@
       <c r="C39" s="4"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" ht="18">
+    <row r="40" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -1046,7 +1053,7 @@
       <c r="C40" s="4"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" ht="18">
+    <row r="41" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -1054,7 +1061,7 @@
       <c r="C41" s="4"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" ht="18">
+    <row r="42" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -1062,7 +1069,7 @@
       <c r="C42" s="4"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" ht="18">
+    <row r="43" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -1070,7 +1077,7 @@
       <c r="C43" s="4"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="18">
+    <row r="44" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -1078,7 +1085,7 @@
       <c r="C44" s="4"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="18">
+    <row r="45" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -1086,7 +1093,7 @@
       <c r="C45" s="4"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="18">
+    <row r="46" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -1094,7 +1101,7 @@
       <c r="C46" s="4"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" ht="18">
+    <row r="47" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -1102,7 +1109,7 @@
       <c r="C47" s="4"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" ht="18">
+    <row r="48" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>46</v>
       </c>
@@ -1110,7 +1117,7 @@
       <c r="C48" s="4"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" ht="18">
+    <row r="49" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -1118,7 +1125,7 @@
       <c r="C49" s="4"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" ht="18">
+    <row r="50" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -1126,7 +1133,7 @@
       <c r="C50" s="4"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" ht="18">
+    <row r="51" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -1134,7 +1141,7 @@
       <c r="C51" s="4"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" ht="18">
+    <row r="52" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -1142,79 +1149,79 @@
       <c r="C52" s="4"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" ht="18">
+    <row r="53" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" ht="18">
+    <row r="54" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" ht="18">
+    <row r="55" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" ht="18">
+    <row r="56" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" ht="18">
+    <row r="57" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4" ht="18">
+    <row r="58" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4" ht="18">
+    <row r="59" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" ht="18">
+    <row r="60" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4" ht="18">
+    <row r="61" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4" ht="18">
+    <row r="62" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" ht="18">
+    <row r="63" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" ht="18">
+    <row r="64" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4" ht="18">
+    <row r="65" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>

</xml_diff>